<commit_message>
Added Analysis for State of Georgia
</commit_message>
<xml_diff>
--- a/2020-03-29-Aggregated.xlsx
+++ b/2020-03-29-Aggregated.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="US Totals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GA Totals" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -355,6 +357,1850 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Infected</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Avaerage (7-Day)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01-22-2020</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01-23-2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f>(B3/B2) - 1</f>
+        <v/>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>01-24-2020</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <f>(B4/B3) - 1</f>
+        <v/>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01-25-2020</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <f>(B5/B4) - 1</f>
+        <v/>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01-26-2020</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>(B6/B5) - 1</f>
+        <v/>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01-27-2020</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <f>(B7/B6) - 1</f>
+        <v/>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01-28-2020</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <f>(B8/B7) - 1</f>
+        <v/>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01-29-2020</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <f>(B9/B8) - 1</f>
+        <v/>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01-30-2020</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <f>(B10/B9) - 1</f>
+        <v/>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01-31-2020</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <f>(B11/B10) - 1</f>
+        <v/>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02-01-2020</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <f>(B12/B11) - 1</f>
+        <v/>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>02-02-2020</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <f>(B13/B12) - 1</f>
+        <v/>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>02-03-2020</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <f>(B14/B13) - 1</f>
+        <v/>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>02-04-2020</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1">
+        <f>(B15/B14) - 1</f>
+        <v/>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>02-05-2020</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <f>(B16/B15) - 1</f>
+        <v/>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>02-06-2020</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
+        <f>(B17/B16) - 1</f>
+        <v/>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>02-07-2020</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <f>(B18/B17) - 1</f>
+        <v/>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>02-08-2020</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <f>(B19/B18) - 1</f>
+        <v/>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>02-09-2020</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
+        <f>(B20/B19) - 1</f>
+        <v/>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>02-10-2020</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
+        <f>(B21/B20) - 1</f>
+        <v/>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>02-11-2020</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1">
+        <f>(B22/B21) - 1</f>
+        <v/>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>02-12-2020</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <f>(B23/B22) - 1</f>
+        <v/>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>02-13-2020</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1">
+        <f>(B24/B23) - 1</f>
+        <v/>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>02-14-2020</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <f>(B25/B24) - 1</f>
+        <v/>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>02-15-2020</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
+        <f>(B26/B25) - 1</f>
+        <v/>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>02-16-2020</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1">
+        <f>(B27/B26) - 1</f>
+        <v/>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>02-17-2020</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1">
+        <f>(B28/B27) - 1</f>
+        <v/>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>02-18-2020</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1">
+        <f>(B29/B28) - 1</f>
+        <v/>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>02-19-2020</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1">
+        <f>(B30/B29) - 1</f>
+        <v/>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>02-20-2020</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1">
+        <f>(B31/B30) - 1</f>
+        <v/>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>02-21-2020</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1">
+        <f>(B32/B31) - 1</f>
+        <v/>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>02-22-2020</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1">
+        <f>(B33/B32) - 1</f>
+        <v/>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>02-23-2020</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>35</v>
+      </c>
+      <c r="C34" s="1">
+        <f>(B34/B33) - 1</f>
+        <v/>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>02-24-2020</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>53</v>
+      </c>
+      <c r="C35" s="1">
+        <f>(B35/B34) - 1</f>
+        <v/>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>02-25-2020</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1">
+        <f>(B36/B35) - 1</f>
+        <v/>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>02-26-2020</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>59</v>
+      </c>
+      <c r="C37" s="1">
+        <f>(B37/B36) - 1</f>
+        <v/>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>02-27-2020</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>60</v>
+      </c>
+      <c r="C38" s="1">
+        <f>(B38/B37) - 1</f>
+        <v/>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>02-28-2020</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>62</v>
+      </c>
+      <c r="C39" s="1">
+        <f>(B39/B38) - 1</f>
+        <v/>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>02-29-2020</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1">
+        <f>(B40/B39) - 1</f>
+        <v/>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>03-01-2020</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>76</v>
+      </c>
+      <c r="C41" s="1">
+        <f>(B41/B40) - 1</f>
+        <v/>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <f>(D41/D40) - 1</f>
+        <v/>
+      </c>
+      <c r="F41" s="1">
+        <f>AVERAGE(E35:E41)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>03-02-2020</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>101</v>
+      </c>
+      <c r="C42" s="1">
+        <f>(B42/B41) - 1</f>
+        <v/>
+      </c>
+      <c r="D42" t="n">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1">
+        <f>(D42/D41) - 1</f>
+        <v/>
+      </c>
+      <c r="F42" s="1">
+        <f>AVERAGE(E36:E42)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>03-03-2020</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>122</v>
+      </c>
+      <c r="C43" s="1">
+        <f>(B43/B42) - 1</f>
+        <v/>
+      </c>
+      <c r="D43" t="n">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1">
+        <f>(D43/D42) - 1</f>
+        <v/>
+      </c>
+      <c r="F43" s="1">
+        <f>AVERAGE(E37:E43)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>03-04-2020</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>153</v>
+      </c>
+      <c r="C44" s="1">
+        <f>(B44/B43) - 1</f>
+        <v/>
+      </c>
+      <c r="D44" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1">
+        <f>(D44/D43) - 1</f>
+        <v/>
+      </c>
+      <c r="F44" s="1">
+        <f>AVERAGE(E38:E44)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>03-05-2020</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>221</v>
+      </c>
+      <c r="C45" s="1">
+        <f>(B45/B44) - 1</f>
+        <v/>
+      </c>
+      <c r="D45" t="n">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1">
+        <f>(D45/D44) - 1</f>
+        <v/>
+      </c>
+      <c r="F45" s="1">
+        <f>AVERAGE(E39:E45)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>03-06-2020</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>278</v>
+      </c>
+      <c r="C46" s="1">
+        <f>(B46/B45) - 1</f>
+        <v/>
+      </c>
+      <c r="D46" t="n">
+        <v>14</v>
+      </c>
+      <c r="E46" s="1">
+        <f>(D46/D45) - 1</f>
+        <v/>
+      </c>
+      <c r="F46" s="1">
+        <f>AVERAGE(E40:E46)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>03-07-2020</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>417</v>
+      </c>
+      <c r="C47" s="1">
+        <f>(B47/B46) - 1</f>
+        <v/>
+      </c>
+      <c r="D47" t="n">
+        <v>17</v>
+      </c>
+      <c r="E47" s="1">
+        <f>(D47/D46) - 1</f>
+        <v/>
+      </c>
+      <c r="F47" s="1">
+        <f>AVERAGE(E41:E47)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>03-08-2020</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>537</v>
+      </c>
+      <c r="C48" s="1">
+        <f>(B48/B47) - 1</f>
+        <v/>
+      </c>
+      <c r="D48" t="n">
+        <v>21</v>
+      </c>
+      <c r="E48" s="1">
+        <f>(D48/D47) - 1</f>
+        <v/>
+      </c>
+      <c r="F48" s="1">
+        <f>AVERAGE(E42:E48)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>03-09-2020</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>605</v>
+      </c>
+      <c r="C49" s="1">
+        <f>(B49/B48) - 1</f>
+        <v/>
+      </c>
+      <c r="D49" t="n">
+        <v>22</v>
+      </c>
+      <c r="E49" s="1">
+        <f>(D49/D48) - 1</f>
+        <v/>
+      </c>
+      <c r="F49" s="1">
+        <f>AVERAGE(E43:E49)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>03-10-2020</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>959</v>
+      </c>
+      <c r="C50" s="1">
+        <f>(B50/B49) - 1</f>
+        <v/>
+      </c>
+      <c r="D50" t="n">
+        <v>28</v>
+      </c>
+      <c r="E50" s="1">
+        <f>(D50/D49) - 1</f>
+        <v/>
+      </c>
+      <c r="F50" s="1">
+        <f>AVERAGE(E44:E50)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>03-11-2020</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1281</v>
+      </c>
+      <c r="C51" s="1">
+        <f>(B51/B50) - 1</f>
+        <v/>
+      </c>
+      <c r="D51" t="n">
+        <v>36</v>
+      </c>
+      <c r="E51" s="1">
+        <f>(D51/D50) - 1</f>
+        <v/>
+      </c>
+      <c r="F51" s="1">
+        <f>AVERAGE(E45:E51)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>03-12-2020</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1663</v>
+      </c>
+      <c r="C52" s="1">
+        <f>(B52/B51) - 1</f>
+        <v/>
+      </c>
+      <c r="D52" t="n">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1">
+        <f>(D52/D51) - 1</f>
+        <v/>
+      </c>
+      <c r="F52" s="1">
+        <f>AVERAGE(E46:E52)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>03-13-2020</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2179</v>
+      </c>
+      <c r="C53" s="1">
+        <f>(B53/B52) - 1</f>
+        <v/>
+      </c>
+      <c r="D53" t="n">
+        <v>47</v>
+      </c>
+      <c r="E53" s="1">
+        <f>(D53/D52) - 1</f>
+        <v/>
+      </c>
+      <c r="F53" s="1">
+        <f>AVERAGE(E47:E53)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>03-14-2020</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2726</v>
+      </c>
+      <c r="C54" s="1">
+        <f>(B54/B53) - 1</f>
+        <v/>
+      </c>
+      <c r="D54" t="n">
+        <v>54</v>
+      </c>
+      <c r="E54" s="1">
+        <f>(D54/D53) - 1</f>
+        <v/>
+      </c>
+      <c r="F54" s="1">
+        <f>AVERAGE(E48:E54)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>03-15-2020</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>3499</v>
+      </c>
+      <c r="C55" s="1">
+        <f>(B55/B54) - 1</f>
+        <v/>
+      </c>
+      <c r="D55" t="n">
+        <v>63</v>
+      </c>
+      <c r="E55" s="1">
+        <f>(D55/D54) - 1</f>
+        <v/>
+      </c>
+      <c r="F55" s="1">
+        <f>AVERAGE(E49:E55)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>03-16-2020</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>4632</v>
+      </c>
+      <c r="C56" s="1">
+        <f>(B56/B55) - 1</f>
+        <v/>
+      </c>
+      <c r="D56" t="n">
+        <v>85</v>
+      </c>
+      <c r="E56" s="1">
+        <f>(D56/D55) - 1</f>
+        <v/>
+      </c>
+      <c r="F56" s="1">
+        <f>AVERAGE(E50:E56)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>03-17-2020</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>6421</v>
+      </c>
+      <c r="C57" s="1">
+        <f>(B57/B56) - 1</f>
+        <v/>
+      </c>
+      <c r="D57" t="n">
+        <v>108</v>
+      </c>
+      <c r="E57" s="1">
+        <f>(D57/D56) - 1</f>
+        <v/>
+      </c>
+      <c r="F57" s="1">
+        <f>AVERAGE(E51:E57)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03-18-2020</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>7786</v>
+      </c>
+      <c r="C58" s="1">
+        <f>(B58/B57) - 1</f>
+        <v/>
+      </c>
+      <c r="D58" t="n">
+        <v>118</v>
+      </c>
+      <c r="E58" s="1">
+        <f>(D58/D57) - 1</f>
+        <v/>
+      </c>
+      <c r="F58" s="1">
+        <f>AVERAGE(E52:E58)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>03-19-2020</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>13680</v>
+      </c>
+      <c r="C59" s="1">
+        <f>(B59/B58) - 1</f>
+        <v/>
+      </c>
+      <c r="D59" t="n">
+        <v>200</v>
+      </c>
+      <c r="E59" s="1">
+        <f>(D59/D58) - 1</f>
+        <v/>
+      </c>
+      <c r="F59" s="1">
+        <f>AVERAGE(E53:E59)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>03-20-2020</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>19101</v>
+      </c>
+      <c r="C60" s="1">
+        <f>(B60/B59) - 1</f>
+        <v/>
+      </c>
+      <c r="D60" t="n">
+        <v>244</v>
+      </c>
+      <c r="E60" s="1">
+        <f>(D60/D59) - 1</f>
+        <v/>
+      </c>
+      <c r="F60" s="1">
+        <f>AVERAGE(E54:E60)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>03-21-2020</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>25493</v>
+      </c>
+      <c r="C61" s="1">
+        <f>(B61/B60) - 1</f>
+        <v/>
+      </c>
+      <c r="D61" t="n">
+        <v>307</v>
+      </c>
+      <c r="E61" s="1">
+        <f>(D61/D60) - 1</f>
+        <v/>
+      </c>
+      <c r="F61" s="1">
+        <f>AVERAGE(E55:E61)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>03-22-2020</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>33746</v>
+      </c>
+      <c r="C62" s="1">
+        <f>(B62/B61) - 1</f>
+        <v/>
+      </c>
+      <c r="D62" t="n">
+        <v>427</v>
+      </c>
+      <c r="E62" s="1">
+        <f>(D62/D61) - 1</f>
+        <v/>
+      </c>
+      <c r="F62" s="1">
+        <f>AVERAGE(E56:E62)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>03-23-2020</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>43667</v>
+      </c>
+      <c r="C63" s="1">
+        <f>(B63/B62) - 1</f>
+        <v/>
+      </c>
+      <c r="D63" t="n">
+        <v>552</v>
+      </c>
+      <c r="E63" s="1">
+        <f>(D63/D62) - 1</f>
+        <v/>
+      </c>
+      <c r="F63" s="1">
+        <f>AVERAGE(E57:E63)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>03-24-2020</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>53740</v>
+      </c>
+      <c r="C64" s="1">
+        <f>(B64/B63) - 1</f>
+        <v/>
+      </c>
+      <c r="D64" t="n">
+        <v>706</v>
+      </c>
+      <c r="E64" s="1">
+        <f>(D64/D63) - 1</f>
+        <v/>
+      </c>
+      <c r="F64" s="1">
+        <f>AVERAGE(E58:E64)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>03-25-2020</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>65778</v>
+      </c>
+      <c r="C65" s="1">
+        <f>(B65/B64) - 1</f>
+        <v/>
+      </c>
+      <c r="D65" t="n">
+        <v>942</v>
+      </c>
+      <c r="E65" s="1">
+        <f>(D65/D64) - 1</f>
+        <v/>
+      </c>
+      <c r="F65" s="1">
+        <f>AVERAGE(E59:E65)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>03-26-2020</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>83836</v>
+      </c>
+      <c r="C66" s="1">
+        <f>(B66/B65) - 1</f>
+        <v/>
+      </c>
+      <c r="D66" t="n">
+        <v>1209</v>
+      </c>
+      <c r="E66" s="1">
+        <f>(D66/D65) - 1</f>
+        <v/>
+      </c>
+      <c r="F66" s="1">
+        <f>AVERAGE(E60:E66)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>03-27-2020</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>101657</v>
+      </c>
+      <c r="C67" s="1">
+        <f>(B67/B66) - 1</f>
+        <v/>
+      </c>
+      <c r="D67" t="n">
+        <v>1581</v>
+      </c>
+      <c r="E67" s="1">
+        <f>(D67/D66) - 1</f>
+        <v/>
+      </c>
+      <c r="F67" s="1">
+        <f>AVERAGE(E61:E67)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>03-28-2020</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>121478</v>
+      </c>
+      <c r="C68" s="1">
+        <f>(B68/B67) - 1</f>
+        <v/>
+      </c>
+      <c r="D68" t="n">
+        <v>2026</v>
+      </c>
+      <c r="E68" s="1">
+        <f>(D68/D67) - 1</f>
+        <v/>
+      </c>
+      <c r="F68" s="1">
+        <f>AVERAGE(E62:E68)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Average (7-Day):</t>
+        </is>
+      </c>
+      <c r="C70" s="1">
+        <f>AVERAGE(C62:C68)</f>
+        <v/>
+      </c>
+      <c r="E70" s="1">
+        <f>AVERAGE(E62:E68)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Projections</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>2653.910040437003</v>
+      </c>
+      <c r="E73" s="1" t="n">
+        <v>0.3094768015794669</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Today +1</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>3476.425717044589</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>0.7156959526159921</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Today +2</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>4553.860372802588</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>1.247285291214215</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Today +3</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>5965.220022768502</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>1.944225074037512</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Today +4</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>7813.996698835724</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>2.856367226061205</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Today +5</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>10235.75730255761</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>4.05182625863771</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Today +6</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>13408.08444063871</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>5.617966436327739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
@@ -400,7 +2246,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -426,11 +2272,12 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <f>(B3/B2) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -451,11 +2298,12 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <f>(B4/B3) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -476,11 +2324,12 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <f>(B5/B4) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -501,11 +2350,12 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <f>(B6/B5) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -526,11 +2376,12 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <f>(B7/B6) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -551,11 +2402,12 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <f>(B8/B7) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -576,11 +2428,12 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
-        <f>(B9/B8) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -601,11 +2454,12 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1">
-        <f>(B10/B9) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -626,11 +2480,12 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1">
-        <f>(B11/B10) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -651,11 +2506,12 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <f>(B12/B11) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -676,11 +2532,12 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <f>(B13/B12) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -701,11 +2558,12 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1">
-        <f>(B14/B13) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -726,11 +2584,12 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1">
-        <f>(B15/B14) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -751,11 +2610,12 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <f>(B16/B15) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -776,11 +2636,12 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1">
-        <f>(B17/B16) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -801,11 +2662,12 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1">
-        <f>(B18/B17) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -826,11 +2688,12 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1">
-        <f>(B19/B18) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -851,11 +2714,12 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1">
-        <f>(B20/B19) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -876,11 +2740,12 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12</v>
-      </c>
-      <c r="C21" s="1">
-        <f>(B21/B20) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -901,11 +2766,12 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1">
-        <f>(B22/B21) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -926,11 +2792,12 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1">
-        <f>(B23/B22) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -951,11 +2818,12 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1">
-        <f>(B24/B23) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -976,11 +2844,12 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1">
-        <f>(B25/B24) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1001,11 +2870,12 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1">
-        <f>(B26/B25) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1026,11 +2896,12 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>15</v>
-      </c>
-      <c r="C27" s="1">
-        <f>(B27/B26) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1051,11 +2922,12 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1">
-        <f>(B28/B27) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1076,11 +2948,12 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1">
-        <f>(B29/B28) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1101,11 +2974,12 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>15</v>
-      </c>
-      <c r="C30" s="1">
-        <f>(B30/B29) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1126,11 +3000,12 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1">
-        <f>(B31/B30) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1151,11 +3026,12 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>35</v>
-      </c>
-      <c r="C32" s="1">
-        <f>(B32/B31) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1176,11 +3052,12 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>35</v>
-      </c>
-      <c r="C33" s="1">
-        <f>(B33/B32) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D33" t="n">
         <v>0</v>
@@ -1201,11 +3078,12 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>35</v>
-      </c>
-      <c r="C34" s="1">
-        <f>(B34/B33) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -1226,11 +3104,12 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>53</v>
-      </c>
-      <c r="C35" s="1">
-        <f>(B35/B34) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D35" t="n">
         <v>0</v>
@@ -1251,11 +3130,12 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>53</v>
-      </c>
-      <c r="C36" s="1">
-        <f>(B36/B35) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -1276,11 +3156,12 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>59</v>
-      </c>
-      <c r="C37" s="1">
-        <f>(B37/B36) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -1301,11 +3182,12 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>60</v>
-      </c>
-      <c r="C38" s="1">
-        <f>(B38/B37) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1326,11 +3208,12 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>62</v>
-      </c>
-      <c r="C39" s="1">
-        <f>(B39/B38) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -1351,14 +3234,15 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>70</v>
-      </c>
-      <c r="C40" s="1">
-        <f>(B40/B39) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1376,22 +3260,23 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>76</v>
-      </c>
-      <c r="C41" s="1">
-        <f>(B41/B40) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
-        <f>(D41/D40) - 1</f>
-        <v/>
-      </c>
-      <c r="F41" s="1">
-        <f>AVERAGE(E35:E41)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1401,22 +3286,23 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1">
-        <f>(B42/B41) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
-      </c>
-      <c r="E42" s="1">
-        <f>(D42/D41) - 1</f>
-        <v/>
-      </c>
-      <c r="F42" s="1">
-        <f>AVERAGE(E36:E42)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1426,22 +3312,23 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>122</v>
-      </c>
-      <c r="C43" s="1">
-        <f>(B43/B42) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
-      </c>
-      <c r="E43" s="1">
-        <f>(D43/D42) - 1</f>
-        <v/>
-      </c>
-      <c r="F43" s="1">
-        <f>AVERAGE(E37:E43)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1451,22 +3338,23 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>153</v>
-      </c>
-      <c r="C44" s="1">
-        <f>(B44/B43) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D44" t="n">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1">
-        <f>(D44/D43) - 1</f>
-        <v/>
-      </c>
-      <c r="F44" s="1">
-        <f>AVERAGE(E38:E44)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1476,22 +3364,23 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>221</v>
-      </c>
-      <c r="C45" s="1">
-        <f>(B45/B44) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D45" t="n">
-        <v>12</v>
-      </c>
-      <c r="E45" s="1">
-        <f>(D45/D44) - 1</f>
-        <v/>
-      </c>
-      <c r="F45" s="1">
-        <f>AVERAGE(E39:E45)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1501,22 +3390,23 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>278</v>
-      </c>
-      <c r="C46" s="1">
-        <f>(B46/B45) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D46" t="n">
-        <v>14</v>
-      </c>
-      <c r="E46" s="1">
-        <f>(D46/D45) - 1</f>
-        <v/>
-      </c>
-      <c r="F46" s="1">
-        <f>AVERAGE(E40:E46)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1526,22 +3416,23 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>417</v>
-      </c>
-      <c r="C47" s="1">
-        <f>(B47/B46) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D47" t="n">
-        <v>17</v>
-      </c>
-      <c r="E47" s="1">
-        <f>(D47/D46) - 1</f>
-        <v/>
-      </c>
-      <c r="F47" s="1">
-        <f>AVERAGE(E41:E47)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1551,22 +3442,23 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>537</v>
-      </c>
-      <c r="C48" s="1">
-        <f>(B48/B47) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D48" t="n">
-        <v>21</v>
-      </c>
-      <c r="E48" s="1">
-        <f>(D48/D47) - 1</f>
-        <v/>
-      </c>
-      <c r="F48" s="1">
-        <f>AVERAGE(E42:E48)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1576,22 +3468,23 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>605</v>
-      </c>
-      <c r="C49" s="1">
-        <f>(B49/B48) - 1</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D49" t="n">
-        <v>22</v>
-      </c>
-      <c r="E49" s="1">
-        <f>(D49/D48) - 1</f>
-        <v/>
-      </c>
-      <c r="F49" s="1">
-        <f>AVERAGE(E43:E49)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1601,22 +3494,23 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>959</v>
-      </c>
-      <c r="C50" s="1">
-        <f>(B50/B49) - 1</f>
-        <v/>
+        <v>17</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
       </c>
       <c r="D50" t="n">
-        <v>28</v>
-      </c>
-      <c r="E50" s="1">
-        <f>(D50/D49) - 1</f>
-        <v/>
-      </c>
-      <c r="F50" s="1">
-        <f>AVERAGE(E44:E50)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1626,22 +3520,22 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1281</v>
+        <v>23</v>
       </c>
       <c r="C51" s="1">
         <f>(B51/B50) - 1</f>
         <v/>
       </c>
       <c r="D51" t="n">
-        <v>36</v>
-      </c>
-      <c r="E51" s="1">
-        <f>(D51/D50) - 1</f>
-        <v/>
-      </c>
-      <c r="F51" s="1">
-        <f>AVERAGE(E45:E51)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1651,22 +3545,22 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1663</v>
+        <v>31</v>
       </c>
       <c r="C52" s="1">
         <f>(B52/B51) - 1</f>
         <v/>
       </c>
       <c r="D52" t="n">
-        <v>40</v>
-      </c>
-      <c r="E52" s="1">
-        <f>(D52/D51) - 1</f>
-        <v/>
-      </c>
-      <c r="F52" s="1">
-        <f>AVERAGE(E46:E52)</f>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>UNDEF</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1676,14 +3570,14 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2179</v>
+        <v>42</v>
       </c>
       <c r="C53" s="1">
         <f>(B53/B52) - 1</f>
         <v/>
       </c>
       <c r="D53" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1">
         <f>(D53/D52) - 1</f>
@@ -1701,14 +3595,14 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2726</v>
+        <v>66</v>
       </c>
       <c r="C54" s="1">
         <f>(B54/B53) - 1</f>
         <v/>
       </c>
       <c r="D54" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="E54" s="1">
         <f>(D54/D53) - 1</f>
@@ -1726,14 +3620,14 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>3499</v>
+        <v>99</v>
       </c>
       <c r="C55" s="1">
         <f>(B55/B54) - 1</f>
         <v/>
       </c>
       <c r="D55" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1">
         <f>(D55/D54) - 1</f>
@@ -1751,14 +3645,14 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>4632</v>
+        <v>121</v>
       </c>
       <c r="C56" s="1">
         <f>(B56/B55) - 1</f>
         <v/>
       </c>
       <c r="D56" t="n">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="E56" s="1">
         <f>(D56/D55) - 1</f>
@@ -1776,14 +3670,14 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6421</v>
+        <v>146</v>
       </c>
       <c r="C57" s="1">
         <f>(B57/B56) - 1</f>
         <v/>
       </c>
       <c r="D57" t="n">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="E57" s="1">
         <f>(D57/D56) - 1</f>
@@ -1801,14 +3695,14 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>7786</v>
+        <v>199</v>
       </c>
       <c r="C58" s="1">
         <f>(B58/B57) - 1</f>
         <v/>
       </c>
       <c r="D58" t="n">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="E58" s="1">
         <f>(D58/D57) - 1</f>
@@ -1826,14 +3720,14 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>13680</v>
+        <v>287</v>
       </c>
       <c r="C59" s="1">
         <f>(B59/B58) - 1</f>
         <v/>
       </c>
       <c r="D59" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="E59" s="1">
         <f>(D59/D58) - 1</f>
@@ -1851,14 +3745,14 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>19101</v>
+        <v>420</v>
       </c>
       <c r="C60" s="1">
         <f>(B60/B59) - 1</f>
         <v/>
       </c>
       <c r="D60" t="n">
-        <v>244</v>
+        <v>13</v>
       </c>
       <c r="E60" s="1">
         <f>(D60/D59) - 1</f>
@@ -1876,14 +3770,14 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>25493</v>
+        <v>507</v>
       </c>
       <c r="C61" s="1">
         <f>(B61/B60) - 1</f>
         <v/>
       </c>
       <c r="D61" t="n">
-        <v>307</v>
+        <v>14</v>
       </c>
       <c r="E61" s="1">
         <f>(D61/D60) - 1</f>
@@ -1901,14 +3795,14 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>33746</v>
+        <v>621</v>
       </c>
       <c r="C62" s="1">
         <f>(B62/B61) - 1</f>
         <v/>
       </c>
       <c r="D62" t="n">
-        <v>427</v>
+        <v>25</v>
       </c>
       <c r="E62" s="1">
         <f>(D62/D61) - 1</f>
@@ -1926,14 +3820,14 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>43667</v>
+        <v>772</v>
       </c>
       <c r="C63" s="1">
         <f>(B63/B62) - 1</f>
         <v/>
       </c>
       <c r="D63" t="n">
-        <v>552</v>
+        <v>25</v>
       </c>
       <c r="E63" s="1">
         <f>(D63/D62) - 1</f>
@@ -1951,14 +3845,14 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>53740</v>
+        <v>1026</v>
       </c>
       <c r="C64" s="1">
         <f>(B64/B63) - 1</f>
         <v/>
       </c>
       <c r="D64" t="n">
-        <v>706</v>
+        <v>32</v>
       </c>
       <c r="E64" s="1">
         <f>(D64/D63) - 1</f>
@@ -1976,14 +3870,14 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>65778</v>
+        <v>1247</v>
       </c>
       <c r="C65" s="1">
         <f>(B65/B64) - 1</f>
         <v/>
       </c>
       <c r="D65" t="n">
-        <v>942</v>
+        <v>40</v>
       </c>
       <c r="E65" s="1">
         <f>(D65/D64) - 1</f>
@@ -2001,14 +3895,14 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>83836</v>
+        <v>1525</v>
       </c>
       <c r="C66" s="1">
         <f>(B66/B65) - 1</f>
         <v/>
       </c>
       <c r="D66" t="n">
-        <v>1209</v>
+        <v>48</v>
       </c>
       <c r="E66" s="1">
         <f>(D66/D65) - 1</f>
@@ -2026,14 +3920,14 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>101657</v>
+        <v>2000</v>
       </c>
       <c r="C67" s="1">
         <f>(B67/B66) - 1</f>
         <v/>
       </c>
       <c r="D67" t="n">
-        <v>1581</v>
+        <v>64</v>
       </c>
       <c r="E67" s="1">
         <f>(D67/D66) - 1</f>
@@ -2051,14 +3945,14 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>121478</v>
+        <v>2366</v>
       </c>
       <c r="C68" s="1">
         <f>(B68/B67) - 1</f>
         <v/>
       </c>
       <c r="D68" t="n">
-        <v>2026</v>
+        <v>69</v>
       </c>
       <c r="E68" s="1">
         <f>(D68/D67) - 1</f>
@@ -2098,10 +3992,10 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>2653.910040437003</v>
+        <v>87.99641581632653</v>
       </c>
       <c r="E73" s="1" t="n">
-        <v>0.3094768015794669</v>
+        <v>0.2608695652173914</v>
       </c>
     </row>
     <row r="74">
@@ -2111,10 +4005,10 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>3476.425717044589</v>
+        <v>112.2227419785484</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.7156959526159921</v>
+        <v>0.6231884057971016</v>
       </c>
     </row>
     <row r="75">
@@ -2124,10 +4018,10 @@
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>4553.860372802588</v>
+        <v>143.1188270607634</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>1.247285291214215</v>
+        <v>1.072463768115942</v>
       </c>
     </row>
     <row r="76">
@@ -2137,10 +4031,10 @@
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>5965.220022768502</v>
+        <v>182.5209248867226</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.944225074037512</v>
+        <v>1.63768115942029</v>
       </c>
     </row>
     <row r="77">
@@ -2150,10 +4044,10 @@
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>7813.996698835724</v>
+        <v>232.7708290074281</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>2.856367226061205</v>
+        <v>2.36231884057971</v>
       </c>
     </row>
     <row r="78">
@@ -2163,10 +4057,10 @@
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>10235.75730255761</v>
+        <v>296.8550530325897</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>4.05182625863771</v>
+        <v>3.289855072463769</v>
       </c>
     </row>
     <row r="79">
@@ -2176,13 +4070,31 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>13408.08444063871</v>
+        <v>378.5823287512091</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>5.617966436327739</v>
+        <v>4.478260869565218</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
20200329 - Initial Update
</commit_message>
<xml_diff>
--- a/2020-03-29-Aggregated.xlsx
+++ b/2020-03-29-Aggregated.xlsx
@@ -357,7 +357,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2077,117 +2077,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>140886</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>2467</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>2653.910040437003</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.3094768015794669</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>3476.425717044589</v>
+        <v>3170.543530407662</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.7156959526159921</v>
+        <v>0.284961491690312</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>4553.860372802588</v>
+        <v>4074.724879695938</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>1.247285291214215</v>
+        <v>0.6513984596676126</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>5965.220022768502</v>
+        <v>5236.762304625495</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.944225074037512</v>
+        <v>1.122415889744629</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>7813.996698835724</v>
+        <v>6730.191668104208</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>2.856367226061205</v>
+        <v>1.728009728415079</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>10235.75730255761</v>
+        <v>8649.519923677075</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>4.05182625863771</v>
+        <v>2.505877584110255</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>13408.08444063871</v>
+        <v>11116.20568915546</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>5.617966436327739</v>
+        <v>3.505877584110255</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>14286.34537107122</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>4.790839075800568</v>
       </c>
     </row>
   </sheetData>
@@ -2201,7 +2226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3969,117 +3994,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>80</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>87.99641581632653</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.2608695652173914</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>112.2227419785484</v>
+        <v>94.86718426501037</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.6231884057971016</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>143.1188270607634</v>
+        <v>112.4972831296429</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>1.072463768115942</v>
+        <v>0.3999999999999999</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>182.5209248867226</v>
+        <v>133.4037560996609</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.63768115942029</v>
+        <v>0.6625000000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>232.7708290074281</v>
+        <v>158.1954838943879</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>2.36231884057971</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>296.8550530325897</v>
+        <v>187.5945015062672</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>3.289855072463769</v>
+        <v>1.3375</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>378.5823287512091</v>
+        <v>222.4570267687227</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>4.478260869565218</v>
+        <v>1.775</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>263.7983968689346</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>2.2875</v>
       </c>
     </row>
   </sheetData>
@@ -4093,7 +4143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5861,117 +5911,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>774</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>16</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>19.18001046572475</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.2666666666666666</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>24.52485343102074</v>
+        <v>20.61105878248735</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>31.35912969848956</v>
+        <v>26.55098400844682</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>1.066666666666667</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>40.09789572086997</v>
+        <v>34.2027432581862</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.666666666666667</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>51.27187063865505</v>
+        <v>44.05967198854992</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>65.55966769644597</v>
+        <v>56.75728058081963</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>3.333333333333333</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>83.82900750315137</v>
+        <v>73.11422789908758</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>4.533333333333333</v>
+        <v>3.5625</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>94.18510306651694</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>4.875</v>
       </c>
     </row>
   </sheetData>
@@ -5985,7 +6060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7753,117 +7828,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>59648</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>965</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>1049.130853472782</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.4409340659340659</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>1511.916961138088</v>
+        <v>1304.589857772497</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>1.075549450549451</v>
+        <v>0.3512953367875649</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>2178.84441183898</v>
+        <v>1763.683623837164</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>1.991758241758242</v>
+        <v>0.8269430051813471</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>3139.962771122295</v>
+        <v>2384.335510857417</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>3.311813186813187</v>
+        <v>1.470466321243523</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>4525.043711456449</v>
+        <v>3223.398886001442</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>5.21565934065934</v>
+        <v>2.339896373056995</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>6521.102982145536</v>
+        <v>4357.734190914659</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>7.957417582417582</v>
+        <v>3.515025906735751</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>9397.651562145948</v>
+        <v>5891.249563042177</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>11.90796703296703</v>
+        <v>5.104663212435233</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>7964.419097980806</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>7.252849740932643</v>
       </c>
     </row>
   </sheetData>
@@ -7877,7 +7977,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9645,45 +9745,57 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1191</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>-1</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
@@ -9696,7 +9808,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
@@ -9709,7 +9821,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
@@ -9722,7 +9834,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
@@ -9735,7 +9847,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
@@ -9748,13 +9860,26 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E79" s="1" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -9769,7 +9894,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11527,117 +11652,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>4465</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>198</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>207.8296111745271</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.1010638297872339</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>229.7507834093358</v>
+        <v>219.4862014345704</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.2180851063829787</v>
+        <v>0.106060606060606</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>253.984127569177</v>
+        <v>243.3040031322061</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>0.3457446808510638</v>
+        <v>0.2272727272727273</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>280.7735238149125</v>
+        <v>269.7064214207714</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>0.4893617021276595</v>
+        <v>0.3585858585858586</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>310.3885759710378</v>
+        <v>298.9739289906898</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>0.6489361702127661</v>
+        <v>0.505050505050505</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>343.1273247716806</v>
+        <v>331.4174343542196</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>0.824468085106383</v>
+        <v>0.6717171717171717</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>379.3192472907132</v>
+        <v>367.3815846242362</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>1.015957446808511</v>
+        <v>0.8535353535353536</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>407.248426697913</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>1.055555555555555</v>
       </c>
     </row>
   </sheetData>
@@ -11651,7 +11801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13419,117 +13569,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>4246</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>56</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>66.90612668547986</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.2222222222222223</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>82.89684792691631</v>
+        <v>69.68042767383098</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.5185185185185186</v>
+        <v>0.2321428571428572</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>102.7093890597263</v>
+        <v>86.70289287157124</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.5357142857142858</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>127.2571740040424</v>
+        <v>107.8838331401685</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.351851851851852</v>
+        <v>0.9107142857142858</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>157.6719371398262</v>
+        <v>134.2391362910564</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>1.907407407407407</v>
+        <v>1.392857142857143</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>195.3559000189302</v>
+        <v>167.0328647736874</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>2.611111111111111</v>
+        <v>1.982142857142857</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>242.0464184337496</v>
+        <v>207.8378830895663</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>3.481481481481482</v>
+        <v>2.696428571428572</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>258.6112960804404</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>3.607142857142857</v>
       </c>
     </row>
   </sheetData>
@@ -13543,7 +13718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15305,117 +15480,142 @@
         <v/>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>5852</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>124</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>Average (7-Day):</t>
         </is>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(C62:C68)</f>
-        <v/>
-      </c>
-      <c r="E70" s="1">
-        <f>AVERAGE(E62:E68)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Projections</t>
-        </is>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Today</t>
-        </is>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>136.8543270493625</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>0.2363636363636363</v>
+          <t>Projections</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Today +1</t>
+          <t>Day +1</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>170.2646075648534</v>
+        <v>152.0981245179827</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.2258064516129032</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Today +2</t>
+          <t>Day +2</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>211.8313480782892</v>
+        <v>186.5632216281271</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>0.9181818181818182</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Today +3</t>
+          <t>Day +3</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>263.5457871746686</v>
+        <v>228.8380331747651</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>1.390909090909091</v>
+        <v>0.8387096774193548</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Today +4</t>
+          <t>Day +4</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>327.885285004398</v>
+        <v>280.6922230989167</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>1.972727272727273</v>
+        <v>1.258064516129032</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Today +5</t>
+          <t>Day +5</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>407.932000260594</v>
+        <v>344.2964572591</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>2.7</v>
+        <v>1.774193548387097</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today +6</t>
+          <t>Day +6</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>507.520539796036</v>
+        <v>422.3132695749587</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>3.609090909090909</v>
+        <v>2.403225806451613</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>518.0085182371649</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>3.17741935483871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Texas and Colorado
</commit_message>
<xml_diff>
--- a/2020-03-29-Aggregated.xlsx
+++ b/2020-03-29-Aggregated.xlsx
@@ -15,7 +15,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WA Totals" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FL Totals" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CA Totals" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TX Totals" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CO Totals" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2220,6 +2222,1941 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Infected</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Avaerage (7-Day)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01-22-2020</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01-23-2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>01-24-2020</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01-25-2020</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01-26-2020</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01-27-2020</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01-28-2020</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01-29-2020</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01-30-2020</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01-31-2020</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02-01-2020</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>02-02-2020</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>02-03-2020</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>02-04-2020</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>02-05-2020</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>02-06-2020</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>02-07-2020</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>02-08-2020</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>02-09-2020</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>02-10-2020</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>02-11-2020</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>02-12-2020</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>02-13-2020</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>02-14-2020</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>02-15-2020</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>02-16-2020</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>02-17-2020</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>02-18-2020</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>02-19-2020</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>02-20-2020</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>02-21-2020</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>02-22-2020</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>02-23-2020</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>02-24-2020</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>02-25-2020</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>02-26-2020</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>02-27-2020</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>02-28-2020</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>02-29-2020</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>03-01-2020</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>03-02-2020</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>03-03-2020</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>03-04-2020</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>03-05-2020</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>03-06-2020</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>03-07-2020</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>03-08-2020</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>03-09-2020</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>03-10-2020</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>15</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>03-11-2020</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>34</v>
+      </c>
+      <c r="C51" s="1">
+        <f>(B51/B50) - 1</f>
+        <v/>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>03-12-2020</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1">
+        <f>(B52/B51) - 1</f>
+        <v/>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>03-13-2020</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>49</v>
+      </c>
+      <c r="C53" s="1">
+        <f>(B53/B52) - 1</f>
+        <v/>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>03-14-2020</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>101</v>
+      </c>
+      <c r="C54" s="1">
+        <f>(B54/B53) - 1</f>
+        <v/>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>03-15-2020</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>131</v>
+      </c>
+      <c r="C55" s="1">
+        <f>(B55/B54) - 1</f>
+        <v/>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <f>(D55/D54) - 1</f>
+        <v/>
+      </c>
+      <c r="F55" s="1">
+        <f>AVERAGE(E49:E55)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>03-16-2020</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>160</v>
+      </c>
+      <c r="C56" s="1">
+        <f>(B56/B55) - 1</f>
+        <v/>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1">
+        <f>(D56/D55) - 1</f>
+        <v/>
+      </c>
+      <c r="F56" s="1">
+        <f>AVERAGE(E50:E56)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>03-17-2020</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>160</v>
+      </c>
+      <c r="C57" s="1">
+        <f>(B57/B56) - 1</f>
+        <v/>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <f>(D57/D56) - 1</f>
+        <v/>
+      </c>
+      <c r="F57" s="1">
+        <f>AVERAGE(E51:E57)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03-18-2020</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>184</v>
+      </c>
+      <c r="C58" s="1">
+        <f>(B58/B57) - 1</f>
+        <v/>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <f>(D58/D57) - 1</f>
+        <v/>
+      </c>
+      <c r="F58" s="1">
+        <f>AVERAGE(E52:E58)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>03-19-2020</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>277</v>
+      </c>
+      <c r="C59" s="1">
+        <f>(B59/B58) - 1</f>
+        <v/>
+      </c>
+      <c r="D59" t="n">
+        <v>4</v>
+      </c>
+      <c r="E59" s="1">
+        <f>(D59/D58) - 1</f>
+        <v/>
+      </c>
+      <c r="F59" s="1">
+        <f>AVERAGE(E53:E59)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>03-20-2020</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>363</v>
+      </c>
+      <c r="C60" s="1">
+        <f>(B60/B59) - 1</f>
+        <v/>
+      </c>
+      <c r="D60" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="1">
+        <f>(D60/D59) - 1</f>
+        <v/>
+      </c>
+      <c r="F60" s="1">
+        <f>AVERAGE(E54:E60)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>03-21-2020</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>390</v>
+      </c>
+      <c r="C61" s="1">
+        <f>(B61/B60) - 1</f>
+        <v/>
+      </c>
+      <c r="D61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" s="1">
+        <f>(D61/D60) - 1</f>
+        <v/>
+      </c>
+      <c r="F61" s="1">
+        <f>AVERAGE(E55:E61)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>03-22-2020</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>591</v>
+      </c>
+      <c r="C62" s="1">
+        <f>(B62/B61) - 1</f>
+        <v/>
+      </c>
+      <c r="D62" t="n">
+        <v>6</v>
+      </c>
+      <c r="E62" s="1">
+        <f>(D62/D61) - 1</f>
+        <v/>
+      </c>
+      <c r="F62" s="1">
+        <f>AVERAGE(E56:E62)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>03-23-2020</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>704</v>
+      </c>
+      <c r="C63" s="1">
+        <f>(B63/B62) - 1</f>
+        <v/>
+      </c>
+      <c r="D63" t="n">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1">
+        <f>(D63/D62) - 1</f>
+        <v/>
+      </c>
+      <c r="F63" s="1">
+        <f>AVERAGE(E57:E63)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>03-24-2020</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>723</v>
+      </c>
+      <c r="C64" s="1">
+        <f>(B64/B63) - 1</f>
+        <v/>
+      </c>
+      <c r="D64" t="n">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1">
+        <f>(D64/D63) - 1</f>
+        <v/>
+      </c>
+      <c r="F64" s="1">
+        <f>AVERAGE(E58:E64)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>03-25-2020</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1021</v>
+      </c>
+      <c r="C65" s="1">
+        <f>(B65/B64) - 1</f>
+        <v/>
+      </c>
+      <c r="D65" t="n">
+        <v>16</v>
+      </c>
+      <c r="E65" s="1">
+        <f>(D65/D64) - 1</f>
+        <v/>
+      </c>
+      <c r="F65" s="1">
+        <f>AVERAGE(E59:E65)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>03-26-2020</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1430</v>
+      </c>
+      <c r="C66" s="1">
+        <f>(B66/B65) - 1</f>
+        <v/>
+      </c>
+      <c r="D66" t="n">
+        <v>19</v>
+      </c>
+      <c r="E66" s="1">
+        <f>(D66/D65) - 1</f>
+        <v/>
+      </c>
+      <c r="F66" s="1">
+        <f>AVERAGE(E60:E66)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>03-27-2020</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1433</v>
+      </c>
+      <c r="C67" s="1">
+        <f>(B67/B66) - 1</f>
+        <v/>
+      </c>
+      <c r="D67" t="n">
+        <v>27</v>
+      </c>
+      <c r="E67" s="1">
+        <f>(D67/D66) - 1</f>
+        <v/>
+      </c>
+      <c r="F67" s="1">
+        <f>AVERAGE(E61:E67)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>03-28-2020</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1740</v>
+      </c>
+      <c r="C68" s="1">
+        <f>(B68/B67) - 1</f>
+        <v/>
+      </c>
+      <c r="D68" t="n">
+        <v>31</v>
+      </c>
+      <c r="E68" s="1">
+        <f>(D68/D67) - 1</f>
+        <v/>
+      </c>
+      <c r="F68" s="1">
+        <f>AVERAGE(E62:E68)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2307</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>47</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Average (7-Day):</t>
+        </is>
+      </c>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Projections</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Day +1</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>64.33866003013165</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>0.3617021276595744</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Day +2</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>88.07368456325234</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>0.8723404255319149</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Day +3</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>120.5647414620457</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>1.553191489361702</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Day +4</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>165.0419981393037</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>2.51063829787234</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Day +5</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>225.9272555101761</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>3.787234042553192</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Day +6</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>309.2735507193598</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>5.574468085106383</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>423.3669326817993</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -15629,14 +17566,1913 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Infected</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Avaerage (7-Day)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01-22-2020</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01-23-2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>01-24-2020</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01-25-2020</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01-26-2020</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01-27-2020</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01-28-2020</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01-29-2020</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01-30-2020</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01-31-2020</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02-01-2020</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>02-02-2020</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>02-03-2020</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>02-04-2020</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>02-05-2020</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>02-06-2020</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>02-07-2020</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>02-08-2020</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>02-09-2020</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>02-10-2020</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>02-11-2020</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>02-12-2020</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>02-13-2020</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>02-14-2020</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>02-15-2020</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>02-16-2020</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>02-17-2020</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>02-18-2020</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>02-19-2020</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>02-20-2020</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>02-21-2020</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>02-22-2020</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>02-23-2020</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>02-24-2020</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>02-25-2020</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>02-26-2020</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>02-27-2020</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>02-28-2020</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>02-29-2020</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>03-01-2020</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>03-02-2020</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>03-03-2020</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>03-04-2020</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>03-05-2020</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>03-06-2020</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>03-07-2020</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>03-08-2020</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>03-09-2020</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>03-10-2020</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>13</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>03-11-2020</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>21</v>
+      </c>
+      <c r="C51" s="1">
+        <f>(B51/B50) - 1</f>
+        <v/>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>03-12-2020</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>27</v>
+      </c>
+      <c r="C52" s="1">
+        <f>(B52/B51) - 1</f>
+        <v/>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>03-13-2020</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>43</v>
+      </c>
+      <c r="C53" s="1">
+        <f>(B53/B52) - 1</f>
+        <v/>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>03-14-2020</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>57</v>
+      </c>
+      <c r="C54" s="1">
+        <f>(B54/B53) - 1</f>
+        <v/>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>03-15-2020</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>72</v>
+      </c>
+      <c r="C55" s="1">
+        <f>(B55/B54) - 1</f>
+        <v/>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>03-16-2020</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>85</v>
+      </c>
+      <c r="C56" s="1">
+        <f>(B56/B55) - 1</f>
+        <v/>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>03-17-2020</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>110</v>
+      </c>
+      <c r="C57" s="1">
+        <f>(B57/B56) - 1</f>
+        <v/>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03-18-2020</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>173</v>
+      </c>
+      <c r="C58" s="1">
+        <f>(B58/B57) - 1</f>
+        <v/>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1">
+        <f>(D58/D57) - 1</f>
+        <v/>
+      </c>
+      <c r="F58" s="1">
+        <f>AVERAGE(E52:E58)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>03-19-2020</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>260</v>
+      </c>
+      <c r="C59" s="1">
+        <f>(B59/B58) - 1</f>
+        <v/>
+      </c>
+      <c r="D59" t="n">
+        <v>5</v>
+      </c>
+      <c r="E59" s="1">
+        <f>(D59/D58) - 1</f>
+        <v/>
+      </c>
+      <c r="F59" s="1">
+        <f>AVERAGE(E53:E59)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>03-20-2020</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>394</v>
+      </c>
+      <c r="C60" s="1">
+        <f>(B60/B59) - 1</f>
+        <v/>
+      </c>
+      <c r="D60" t="n">
+        <v>5</v>
+      </c>
+      <c r="E60" s="1">
+        <f>(D60/D59) - 1</f>
+        <v/>
+      </c>
+      <c r="F60" s="1">
+        <f>AVERAGE(E54:E60)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>03-21-2020</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>581</v>
+      </c>
+      <c r="C61" s="1">
+        <f>(B61/B60) - 1</f>
+        <v/>
+      </c>
+      <c r="D61" t="n">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <f>(D61/D60) - 1</f>
+        <v/>
+      </c>
+      <c r="F61" s="1">
+        <f>AVERAGE(E55:E61)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>03-22-2020</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>643</v>
+      </c>
+      <c r="C62" s="1">
+        <f>(B62/B61) - 1</f>
+        <v/>
+      </c>
+      <c r="D62" t="n">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1">
+        <f>(D62/D61) - 1</f>
+        <v/>
+      </c>
+      <c r="F62" s="1">
+        <f>AVERAGE(E56:E62)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>03-23-2020</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>758</v>
+      </c>
+      <c r="C63" s="1">
+        <f>(B63/B62) - 1</f>
+        <v/>
+      </c>
+      <c r="D63" t="n">
+        <v>9</v>
+      </c>
+      <c r="E63" s="1">
+        <f>(D63/D62) - 1</f>
+        <v/>
+      </c>
+      <c r="F63" s="1">
+        <f>AVERAGE(E57:E63)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>03-24-2020</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>955</v>
+      </c>
+      <c r="C64" s="1">
+        <f>(B64/B63) - 1</f>
+        <v/>
+      </c>
+      <c r="D64" t="n">
+        <v>12</v>
+      </c>
+      <c r="E64" s="1">
+        <f>(D64/D63) - 1</f>
+        <v/>
+      </c>
+      <c r="F64" s="1">
+        <f>AVERAGE(E58:E64)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>03-25-2020</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1229</v>
+      </c>
+      <c r="C65" s="1">
+        <f>(B65/B64) - 1</f>
+        <v/>
+      </c>
+      <c r="D65" t="n">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <f>(D65/D64) - 1</f>
+        <v/>
+      </c>
+      <c r="F65" s="1">
+        <f>AVERAGE(E59:E65)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>03-26-2020</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1563</v>
+      </c>
+      <c r="C66" s="1">
+        <f>(B66/B65) - 1</f>
+        <v/>
+      </c>
+      <c r="D66" t="n">
+        <v>21</v>
+      </c>
+      <c r="E66" s="1">
+        <f>(D66/D65) - 1</f>
+        <v/>
+      </c>
+      <c r="F66" s="1">
+        <f>AVERAGE(E60:E66)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>03-27-2020</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1937</v>
+      </c>
+      <c r="C67" s="1">
+        <f>(B67/B66) - 1</f>
+        <v/>
+      </c>
+      <c r="D67" t="n">
+        <v>26</v>
+      </c>
+      <c r="E67" s="1">
+        <f>(D67/D66) - 1</f>
+        <v/>
+      </c>
+      <c r="F67" s="1">
+        <f>AVERAGE(E61:E67)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>03-28-2020</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2455</v>
+      </c>
+      <c r="C68" s="1">
+        <f>(B68/B67) - 1</f>
+        <v/>
+      </c>
+      <c r="D68" t="n">
+        <v>30</v>
+      </c>
+      <c r="E68" s="1">
+        <f>(D68/D67) - 1</f>
+        <v/>
+      </c>
+      <c r="F68" s="1">
+        <f>AVERAGE(E62:E68)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>03-29-2020</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2792</v>
+      </c>
+      <c r="C69" s="1">
+        <f>(B69/B68) - 1</f>
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v>37</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(D69/D68) - 1</f>
+        <v/>
+      </c>
+      <c r="F69" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Average (7-Day):</t>
+        </is>
+      </c>
+      <c r="C71" s="1">
+        <f>AVERAGE(C63:C69)</f>
+        <v/>
+      </c>
+      <c r="E71" s="1">
+        <f>AVERAGE(E63:E69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Projections</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Day +1</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>47.01284667713239</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>0.2702702702702702</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Day +2</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>59.73534466723129</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>0.5945945945945945</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Day +3</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>75.90077297422168</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>1.027027027027027</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Day +4</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>96.44084871656533</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>1.594594594594595</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Day +5</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>122.5394279493082</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>2.297297297297297</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Day +6</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>155.7007388671443</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>3.189189189189189</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Day +7</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>197.8360801047914</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>4.324324324324325</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>